<commit_message>
return more data from node middleware, c++ server can insert data to index_chinesename
</commit_message>
<xml_diff>
--- a/数据库格式.xlsx
+++ b/数据库格式.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\svn_kai\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git_kai\project\StockData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{851662B5-87D5-479F-B68B-B14B0E134F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44C9A3A-F68C-49D9-BEDE-D9750A4F40BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1440" windowWidth="29040" windowHeight="15840" xr2:uid="{53076C79-76A8-4AE7-B8CE-F32584635617}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53076C79-76A8-4AE7-B8CE-F32584635617}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,16 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>股票代码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>股票中文名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>信息类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -54,6 +50,102 @@
   </si>
   <si>
     <t>（min, day, time）</t>
+  </si>
+  <si>
+    <t>数据库1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stock_day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATOCK_INDEX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHINESE_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT NOT NULL primary key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(200) not null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对应中文名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最高价</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最低价</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始价</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结束价</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成交量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>end</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>trading volume</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stock_day_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -91,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +205,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -131,7 +259,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -148,6 +276,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,106 +619,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7FE86E-2DE3-4CB6-BE36-59AA0DFE3788}">
-  <dimension ref="C2:O16"/>
+  <dimension ref="B2:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="5" max="5" width="17.75" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="N2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
     </row>
     <row r="3" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="2"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4" s="4"/>
       <c r="D4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="2"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C5" s="4"/>
       <c r="D5" s="3"/>
       <c r="E5" s="5"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="2"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C6" s="4"/>
       <c r="D6" s="3"/>
       <c r="E6" s="5"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="2"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
     </row>
     <row r="7" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C7" s="4"/>
       <c r="D7" s="3"/>
       <c r="E7" s="5"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="2"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
       <c r="E8" s="5"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="2"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C9" s="4"/>
       <c r="D9" s="3"/>
       <c r="E9" s="5"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="2"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
     </row>
     <row r="10" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C10" s="4"/>
       <c r="D10" s="3"/>
       <c r="E10" s="5"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="2"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C11" s="4"/>
       <c r="D11" s="3"/>
       <c r="E11" s="5"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="2"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="5"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="2"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="5"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="2"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C14" s="4"/>
@@ -579,6 +734,209 @@
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="5"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="7"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="7"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D28" s="6"/>
+      <c r="E28" s="7"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="7"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="7"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="7"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D32" s="6"/>
+      <c r="E32" s="7"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="7"/>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="D33" s="6"/>
+      <c r="E33" s="7"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="7"/>
+    </row>
+    <row r="37" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C37" s="14"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="14"/>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C38" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="D40" s="3"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="D41" s="3"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="D42" s="3"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="13"/>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="D43" s="3"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="13"/>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="D44" s="3"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
data can insert into DB successfully
</commit_message>
<xml_diff>
--- a/数据库格式.xlsx
+++ b/数据库格式.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git_kai\project\StockData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA04776-9F97-4EC0-92F5-551B22E2102D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B09626A-2CB1-4CA9-BD60-1F41133389F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53076C79-76A8-4AE7-B8CE-F32584635617}"/>
+    <workbookView xWindow="-28920" yWindow="-1440" windowWidth="29040" windowHeight="15840" xr2:uid="{53076C79-76A8-4AE7-B8CE-F32584635617}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>数据库1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -156,42 +156,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MIN_DATE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MIN_STATRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MIN_END</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MIN_MAX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MIN_MIN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MIN_TRAYNING_TOTAL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>其他</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>换手率</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OTHERS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>EXCHANGE_RATIO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -205,6 +177,34 @@
   </si>
   <si>
     <t>stock_min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STATRT_MIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>END_MIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX_MIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANING_TOTAL_MIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期+分钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATEplusMIN_MIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>primary key(ATOCK_INDEX,DAY_DATE)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -243,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,12 +300,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -325,7 +319,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -368,10 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -688,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7FE86E-2DE3-4CB6-BE36-59AA0DFE3788}">
-  <dimension ref="B2:Y44"/>
+  <dimension ref="B2:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="X32" sqref="X32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -801,7 +792,7 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
@@ -812,12 +803,12 @@
         <v>2</v>
       </c>
       <c r="Q22" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C23" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>7</v>
@@ -837,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="R24" s="2" t="s">
         <v>7</v>
@@ -906,17 +897,17 @@
       <c r="R32" s="3"/>
       <c r="S32" s="4"/>
     </row>
-    <row r="33" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:24" x14ac:dyDescent="0.2">
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
       <c r="R33" s="3"/>
       <c r="S33" s="4"/>
     </row>
-    <row r="34" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:24" x14ac:dyDescent="0.2">
       <c r="R34" s="3"/>
       <c r="S34" s="4"/>
     </row>
-    <row r="37" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C37" s="11"/>
       <c r="D37" s="6"/>
       <c r="E37" s="11"/>
@@ -924,7 +915,7 @@
         <v>15</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="S37" s="7" t="s">
         <v>12</v>
@@ -942,13 +933,10 @@
         <v>29</v>
       </c>
       <c r="X37" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y37" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="3:25" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C38" s="5" t="s">
         <v>17</v>
       </c>
@@ -977,31 +965,28 @@
         <v>28</v>
       </c>
       <c r="R38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S38" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T38" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U38" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V38" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="S38" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T38" s="4" t="s">
+      <c r="W38" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="X38" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="U38" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="V38" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="W38" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="X38" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y38" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="3:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>18</v>
       </c>
@@ -1036,9 +1021,8 @@
       <c r="V39" s="9"/>
       <c r="W39" s="10"/>
       <c r="X39" s="14"/>
-      <c r="Y39" s="15"/>
-    </row>
-    <row r="40" spans="3:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>16</v>
       </c>
@@ -1058,9 +1042,8 @@
       <c r="V40" s="9"/>
       <c r="W40" s="10"/>
       <c r="X40" s="14"/>
-      <c r="Y40" s="15"/>
-    </row>
-    <row r="41" spans="3:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="3:24" x14ac:dyDescent="0.2">
       <c r="D41" s="13"/>
       <c r="E41" s="2"/>
       <c r="F41" s="7"/>
@@ -1075,9 +1058,8 @@
       <c r="V41" s="9"/>
       <c r="W41" s="10"/>
       <c r="X41" s="14"/>
-      <c r="Y41" s="15"/>
-    </row>
-    <row r="42" spans="3:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="3:24" x14ac:dyDescent="0.2">
       <c r="D42" s="13"/>
       <c r="E42" s="2"/>
       <c r="F42" s="7"/>
@@ -1092,9 +1074,8 @@
       <c r="V42" s="9"/>
       <c r="W42" s="10"/>
       <c r="X42" s="14"/>
-      <c r="Y42" s="15"/>
-    </row>
-    <row r="43" spans="3:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="3:24" x14ac:dyDescent="0.2">
       <c r="D43" s="13"/>
       <c r="E43" s="2"/>
       <c r="F43" s="7"/>
@@ -1109,9 +1090,8 @@
       <c r="V43" s="9"/>
       <c r="W43" s="10"/>
       <c r="X43" s="14"/>
-      <c r="Y43" s="15"/>
-    </row>
-    <row r="44" spans="3:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="3:24" x14ac:dyDescent="0.2">
       <c r="D44" s="13"/>
       <c r="E44" s="2"/>
       <c r="F44" s="7"/>
@@ -1120,6 +1100,11 @@
       <c r="I44" s="9"/>
       <c r="J44" s="10"/>
     </row>
+    <row r="45" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>